<commit_message>
Updating quantity requested validations
</commit_message>
<xml_diff>
--- a/forms/app/stock_refill_request.xlsx
+++ b/forms/app/stock_refill_request.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -203,6 +203,12 @@
     <t xml:space="preserve">selected(${known_requested_items}, 'ACT')</t>
   </si>
   <si>
+    <t xml:space="preserve">.&gt;=0 and .&lt;100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 100</t>
+  </si>
+  <si>
     <t xml:space="preserve">zinc_quantity_requested</t>
   </si>
   <si>
@@ -210,6 +216,9 @@
   </si>
   <si>
     <t xml:space="preserve">selected(${known_requested_items}, 'zinc')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 101</t>
   </si>
   <si>
     <t xml:space="preserve">amoxicillin_quantity_requested</t>
@@ -246,6 +255,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 102</t>
+  </si>
+  <si>
     <t xml:space="preserve">condoms_quantity_requested</t>
   </si>
   <si>
@@ -280,6 +292,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 103</t>
+  </si>
+  <si>
     <t xml:space="preserve">contraceptives_quantity_requested</t>
   </si>
   <si>
@@ -314,6 +329,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 104</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -362,6 +380,9 @@
       </rPr>
       <t xml:space="preserve">')</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Value should be greater 0 and less than 105</t>
   </si>
   <si>
     <t xml:space="preserve">begin repeat</t>
@@ -629,14 +650,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -741,7 +762,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -795,6 +816,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1072,7 +1097,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1083,6 +1108,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.77"/>
@@ -1776,8 +1802,17 @@
       <c r="C23" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="E23" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,13 +1820,22 @@
         <v>49</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>55</v>
+      <c r="H24" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,13 +1843,22 @@
         <v>49</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,13 +1866,22 @@
         <v>49</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,13 +1889,22 @@
         <v>49</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,47 +1912,59 @@
         <v>49</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>71</v>
+      <c r="E30" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,18 +1972,27 @@
         <v>49</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="14"/>
+        <v>83</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="15"/>
+      <c r="G31" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="14"/>
+        <v>84</v>
+      </c>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" s="12" customFormat="true" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
@@ -1910,11 +2002,11 @@
     <row r="34" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="15"/>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15"/>
-      <c r="E37" s="15"/>
+      <c r="A37" s="16"/>
+      <c r="E37" s="16"/>
     </row>
     <row r="38" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2090,13 +2182,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
@@ -2123,102 +2215,102 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>81</v>
+      <c r="A2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>83</v>
+      <c r="A3" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>85</v>
+      <c r="A4" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>87</v>
+      <c r="B5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>89</v>
+      <c r="A6" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>91</v>
+      <c r="A7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>93</v>
+      <c r="A8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2246,60 +2338,60 @@
   <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
+      <c r="A1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>108</v>
+      <c r="A2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding requesting can be done only once per day validation
</commit_message>
<xml_diff>
--- a/forms/app/stock_refill_request.xlsx
+++ b/forms/app/stock_refill_request.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="203">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -120,6 +120,9 @@
     <t xml:space="preserve">db-object bind-id-only</t>
   </si>
   <si>
+    <t xml:space="preserve">${recently_requested} != ‘true’</t>
+  </si>
+  <si>
     <t xml:space="preserve">Select the family from the list</t>
   </si>
   <si>
@@ -208,6 +211,15 @@
   </si>
   <si>
     <t xml:space="preserve">../inputs/contact/community_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recently_requested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance('contact-summary')/context/recentlyRequested</t>
   </si>
   <si>
     <t xml:space="preserve">is_act_selected</t>
@@ -851,9 +863,6 @@
   </si>
   <si>
     <t xml:space="preserve">other_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO_LABEL</t>
   </si>
   <si>
     <r>
@@ -1152,7 +1161,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1237,6 +1246,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1253,6 +1268,20 @@
       <sz val="14"/>
       <color rgb="FFE36C09"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1347,7 +1376,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1357,13 +1386,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFCC99FF"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDBE5F1"/>
-        <bgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -1375,16 +1422,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FF76A5AF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1417,7 +1479,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1458,11 +1520,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1470,39 +1536,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1514,11 +1600,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1526,27 +1612,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1554,23 +1628,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1584,7 +1670,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -1673,6 +1759,57 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1693,16 +1830,16 @@
       <rgbColor rgb="FF548235"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4A7D6"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC27BA0"/>
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFDBE5F1"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDBE5F1"/>
+      <rgbColor rgb="FFD9D2E9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1715,10 +1852,10 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFB4A7D6"/>
+      <rgbColor rgb="FFEAD1DC"/>
       <rgbColor rgb="FF2F75B5"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
@@ -1726,9 +1863,9 @@
       <rgbColor rgb="FFBF8F00"/>
       <rgbColor rgb="FFE36C09"/>
       <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF76A5AF"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF70AD47"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF833C0C"/>
@@ -1749,17 +1886,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ79"/>
+  <dimension ref="A1:AMJ80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="I58" activeCellId="0" sqref="I58"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.68"/>
@@ -1950,26 +2087,28 @@
       <c r="F6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
     </row>
     <row r="7" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -1979,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1991,29 +2130,29 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
     </row>
     <row r="8" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -2025,29 +2164,29 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
     </row>
     <row r="9" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2059,19 +2198,19 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
     </row>
     <row r="10" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -2111,7 +2250,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -2122,22 +2261,22 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
     </row>
     <row r="12" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
@@ -2147,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2159,23 +2298,23 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
     </row>
     <row r="13" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2206,7 +2345,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2231,34 +2370,34 @@
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" s="13" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+    <row r="15" s="14" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
+      <c r="C15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
     </row>
     <row r="16" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2286,7 +2425,7 @@
     </row>
     <row r="17" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2314,7 +2453,7 @@
     </row>
     <row r="18" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2341,641 +2480,659 @@
       <c r="X18" s="4"/>
     </row>
     <row r="19" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+    </row>
+    <row r="20" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+    </row>
+    <row r="21" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+    </row>
+    <row r="23" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+    </row>
+    <row r="24" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+    </row>
+    <row r="25" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-    </row>
-    <row r="20" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-    </row>
-    <row r="21" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-    </row>
-    <row r="22" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-    </row>
-    <row r="23" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-    </row>
-    <row r="24" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-    </row>
-    <row r="25" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14" t="s">
+      <c r="B25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-    </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="17" t="s">
+      <c r="C25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+    </row>
+    <row r="26" s="21" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16" t="s">
+      <c r="C26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16" t="s">
+      <c r="A27" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
+      <c r="C27" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
+      <c r="A29" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
+      <c r="A30" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16"/>
+      <c r="A31" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
+      <c r="A32" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="16"/>
+      <c r="A33" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
+      <c r="A34" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
+      <c r="A35" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
+      <c r="A36" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-    </row>
-    <row r="38" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="18" t="s">
+      <c r="A37" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+    </row>
+    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
+    </row>
+    <row r="39" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19" t="s">
+      <c r="B39" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="AMH38" s="0"/>
-      <c r="AMI38" s="0"/>
-      <c r="AMJ38" s="0"/>
-    </row>
-    <row r="39" s="18" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="0" t="s">
+    <row r="40" s="24" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="B40" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="25"/>
+      <c r="F40" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>94</v>
       </c>
@@ -2986,156 +3143,147 @@
         <v>96</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F41" s="0" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="B42" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="C42" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="D42" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="22" t="s">
+      <c r="F42" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="D43" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="22" t="s">
+      <c r="G43" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="H43" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="H43" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="B44" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" s="28" t="s">
         <v>108</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>113</v>
+        <v>97</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="H45" s="28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>116</v>
+        <v>97</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>117</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>119</v>
+        <v>97</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="G47" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="H47" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>121</v>
@@ -3143,11 +3291,17 @@
       <c r="C48" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="D48" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="24" t="s">
-        <v>19</v>
+      <c r="G48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,437 +3312,454 @@
         <v>125</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F49" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" s="24"/>
-      <c r="G50" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" s="24"/>
-    </row>
-    <row r="52" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="AMH52" s="0"/>
-      <c r="AMI52" s="0"/>
-      <c r="AMJ52" s="0"/>
-    </row>
-    <row r="53" s="25" customFormat="true" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" s="30"/>
+      <c r="G51" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="30"/>
+    </row>
+    <row r="53" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AMH53" s="0"/>
+      <c r="AMI53" s="0"/>
+      <c r="AMJ53" s="0"/>
+    </row>
+    <row r="54" s="31" customFormat="true" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="N53" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" s="26" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="I54" s="26" t="s">
+      <c r="C54" s="31" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="55" s="26" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="26" t="s">
+      <c r="N54" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" s="32" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" s="32" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I55" s="26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" s="26" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="I56" s="26" t="s">
+      <c r="I56" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" s="32" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" s="32" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="J58" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="O58" s="32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" s="32" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="34"/>
+      <c r="O60" s="34"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="34"/>
+      <c r="R60" s="34"/>
+      <c r="S60" s="34"/>
+      <c r="T60" s="34"/>
+      <c r="U60" s="34"/>
+    </row>
+    <row r="61" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" s="26" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="J57" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="O57" s="26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" s="26" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="I58" s="26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="27" t="s">
+      <c r="R61" s="36"/>
+      <c r="S61" s="36"/>
+      <c r="T61" s="36"/>
+      <c r="U61" s="36"/>
+    </row>
+    <row r="62" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+    </row>
+    <row r="63" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="27"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="28"/>
-      <c r="N59" s="28"/>
-      <c r="O59" s="28"/>
-      <c r="P59" s="28"/>
-      <c r="Q59" s="28"/>
-      <c r="R59" s="28"/>
-      <c r="S59" s="28"/>
-      <c r="T59" s="28"/>
-      <c r="U59" s="28"/>
-    </row>
-    <row r="60" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B60" s="5" t="s">
+      <c r="B63" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
+    </row>
+    <row r="64" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I60" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="R60" s="30"/>
-      <c r="S60" s="30"/>
-      <c r="T60" s="30"/>
-      <c r="U60" s="30"/>
-    </row>
-    <row r="61" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-      <c r="J61" s="31"/>
-      <c r="K61" s="31"/>
-    </row>
-    <row r="62" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="32" t="s">
+      <c r="I64" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+    </row>
+    <row r="66" s="39" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
-    </row>
-    <row r="63" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
-      <c r="J64" s="32"/>
-      <c r="K64" s="32"/>
-    </row>
-    <row r="65" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B65" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="AMI65" s="0"/>
-      <c r="AMJ65" s="0"/>
-    </row>
-    <row r="66" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I66" s="17" t="s">
-        <v>146</v>
+      <c r="B66" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="39" t="s">
+        <v>147</v>
       </c>
       <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I67" s="17" t="s">
+    <row r="67" s="39" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>148</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>149</v>
       </c>
       <c r="AMI67" s="0"/>
       <c r="AMJ67" s="0"/>
     </row>
-    <row r="68" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I68" s="17" t="s">
+    <row r="68" s="39" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="23" t="s">
         <v>150</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>151</v>
       </c>
       <c r="AMI68" s="0"/>
       <c r="AMJ68" s="0"/>
     </row>
-    <row r="69" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I69" s="17" t="s">
+    <row r="69" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="23" t="s">
         <v>152</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I69" s="23" t="s">
+        <v>153</v>
       </c>
       <c r="AMI69" s="0"/>
       <c r="AMJ69" s="0"/>
     </row>
-    <row r="70" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I70" s="17" t="s">
+    <row r="70" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70" s="23" t="s">
         <v>154</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I70" s="23" t="s">
+        <v>155</v>
       </c>
       <c r="AMI70" s="0"/>
       <c r="AMJ70" s="0"/>
     </row>
-    <row r="71" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C71" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I71" s="17" t="s">
+    <row r="71" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>156</v>
+      </c>
+      <c r="C71" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="AMI71" s="0"/>
       <c r="AMJ71" s="0"/>
     </row>
-    <row r="72" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C72" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I72" s="17" t="s">
+    <row r="72" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>158</v>
+      </c>
+      <c r="C72" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="AMI72" s="0"/>
       <c r="AMJ72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="C73" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I73" s="17" t="s">
+    <row r="73" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73" s="23" t="s">
         <v>160</v>
       </c>
+      <c r="C73" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="AMI73" s="0"/>
+      <c r="AMJ73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C74" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I74" s="17" t="s">
+      <c r="A74" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" s="23" t="s">
         <v>162</v>
       </c>
+      <c r="C74" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I74" s="23" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C75" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I75" s="17" t="s">
+      <c r="A75" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="23" t="s">
         <v>164</v>
       </c>
+      <c r="C75" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C76" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I76" s="17" t="s">
+      <c r="A76" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B76" s="23" t="s">
         <v>166</v>
       </c>
+      <c r="C76" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="I77" s="17" t="s">
+      <c r="A77" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" s="23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78" s="17"/>
-      <c r="I78" s="17"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I77" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C78" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I78" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B79" s="23"/>
+      <c r="I79" s="23"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3628,6 +3799,72 @@
       <formula>"begin group"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("calculate",A26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND($A26="begin group", NOT($B26 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND($A26="end group", $B26 = "", $C26 = "", $D26 = "", $E26 = "", $F26 = "", $G26 = "", $H26 = "", $I26 = "", $J26 = "", $K26 = "", $L26 = "", $M26 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>AND($A26="begin repeat", NOT($B26 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:V26">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+      <formula>AND($A26="end repeat", $B26 = "", $C26 = "", $D26 = "", $E26 = "", $F26 = "", $G26 = "", $H26 = "", $I26 = "", $J26 = "", $K26 = "", $L26 = "", $M26 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>AND(AND(NOT($A26 = "end group"), NOT($A26 = "end repeat"), NOT($A26 = "")), $B26 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>COUNTIF($B$2:$B$456,B26)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>AND(AND(NOT($A26 = "end group"), NOT($A26 = "end repeat"), NOT($A26 = "")), $C26 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>AND(NOT($G26 = ""), $H26 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND($I26 = "", $A26 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D26" type="list">
+      <formula1>"yes,no"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3650,7 +3887,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.68"/>
@@ -3659,13 +3896,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="34" t="s">
+      <c r="A1" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
@@ -3692,102 +3929,102 @@
       <c r="Y1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>172</v>
+      <c r="A2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>174</v>
+      <c r="B3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>176</v>
+      <c r="A4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>178</v>
+      <c r="A5" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>180</v>
+      <c r="A6" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>182</v>
+      <c r="A7" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>184</v>
+      <c r="A8" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3812,63 +4049,63 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="35" t="s">
+      <c r="A1" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="B1" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
+      <c r="D1" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>199</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving the form and the task
</commit_message>
<xml_diff>
--- a/forms/app/stock_refill_request.xlsx
+++ b/forms/app/stock_refill_request.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="203">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -207,7 +207,7 @@
     <t xml:space="preserve">../inputs/contact/parent/_id</t>
   </si>
   <si>
-    <t xml:space="preserve">chv_commuity_unit</t>
+    <t xml:space="preserve">chv_community_unit</t>
   </si>
   <si>
     <t xml:space="preserve">../inputs/contact/community_unit</t>
@@ -633,18 +633,8 @@
         <color rgb="FFE36C09"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">chv_commuity_unit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}</t>
+      </rPr>
+      <t xml:space="preserve">chv_area_name}</t>
     </r>
   </si>
   <si>
@@ -1250,6 +1240,7 @@
       <color rgb="FF000000"/>
       <name val="arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1279,13 +1270,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -1310,6 +1294,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFE36C09"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1552,27 +1542,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1580,14 +1570,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1600,7 +1590,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1889,14 +1879,14 @@
   <dimension ref="A1:AMJ80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.68"/>
@@ -3125,9 +3115,7 @@
         <v>93</v>
       </c>
       <c r="E40" s="25"/>
-      <c r="F40" s="27" t="s">
-        <v>30</v>
-      </c>
+      <c r="F40" s="27"/>
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
@@ -3887,7 +3875,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.68"/>
@@ -4049,7 +4037,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">

</xml_diff>